<commit_message>
updated df data structure to include fluorophore properties
</commit_message>
<xml_diff>
--- a/Fluorophores/Fluorophore_Properties.xlsx
+++ b/Fluorophores/Fluorophore_Properties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Documents\Software\Python\SpectralCrosstalkOptimization\Fluorophores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A25AE4E9-A069-4FF3-8DE6-345AA1DA9C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33291D46-67E8-4B8F-A87C-52104994A07C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-870" windowWidth="29040" windowHeight="15720" xr2:uid="{456F020B-E735-48F7-8319-EF6BF7EFDDBE}"/>
   </bookViews>
@@ -59,12 +59,6 @@
     <t>Fluorophore</t>
   </si>
   <si>
-    <t>Quantum Yield</t>
-  </si>
-  <si>
-    <t>Extinction Coefficient (cm⁻¹M⁻¹)</t>
-  </si>
-  <si>
     <t>ATTO488</t>
   </si>
   <si>
@@ -116,13 +110,19 @@
     <t>ATTO-Tec</t>
   </si>
   <si>
-    <t>116,000 </t>
-  </si>
-  <si>
     <t>Birge, R. R. (1987) kodak laser yes</t>
   </si>
   <si>
     <t>Source</t>
+  </si>
+  <si>
+    <t>QE</t>
+  </si>
+  <si>
+    <t>ExtCoeff</t>
+  </si>
+  <si>
+    <t>116000 </t>
   </si>
 </sst>
 </file>
@@ -507,7 +507,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,18 +522,18 @@
         <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>0.75</v>
@@ -542,12 +542,12 @@
         <v>75000</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>0.8</v>
@@ -556,12 +556,12 @@
         <v>90000</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>0.9</v>
@@ -570,12 +570,12 @@
         <v>110000</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>0.9</v>
@@ -584,12 +584,12 @@
         <v>115000</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>0.8</v>
@@ -598,12 +598,12 @@
         <v>120000</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>0.9</v>
@@ -612,12 +612,12 @@
         <v>120000</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>0.8</v>
@@ -626,12 +626,12 @@
         <v>120000</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>0.85</v>
@@ -640,12 +640,12 @@
         <v>120000</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>0.5</v>
@@ -654,12 +654,12 @@
         <v>120000</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>0.65</v>
@@ -668,12 +668,12 @@
         <v>150000</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>0.3</v>
@@ -682,7 +682,7 @@
         <v>125000</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -696,7 +696,7 @@
         <v>74000</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -710,7 +710,7 @@
         <v>150000</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -724,12 +724,12 @@
         <v>250000</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>0.2</v>
@@ -738,7 +738,7 @@
         <v>198000</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -752,12 +752,12 @@
         <v>87770</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>0.61</v>
@@ -766,7 +766,7 @@
         <v>75000</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -780,7 +780,7 @@
         <v>93000</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -794,12 +794,12 @@
         <v>84000</v>
       </c>
       <c r="D20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>0.79</v>
@@ -808,21 +808,21 @@
         <v>98000</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>0.95</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>